<commit_message>
MECAmaster Premiers cas de charges
Cas plutôt extrêmes
</commit_message>
<xml_diff>
--- a/SU_Suspension/05_Cas de charges/Cas de charges Valkyriz.xlsx
+++ b/SU_Suspension/05_Cas de charges/Cas de charges Valkyriz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\05_Cas de charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E985CE98-E5E7-473A-9592-B9ED19D9794A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0102EA-54A5-4ABB-B3DD-A8F05C298C71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E17D21D-D292-4944-904A-D92C97BB235F}"/>
   </bookViews>
@@ -497,35 +497,14 @@
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -535,18 +514,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -562,20 +529,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="20"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,7 +999,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,72 +1014,72 @@
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
+      <c r="A12" s="3"/>
       <c r="F12" t="s">
         <v>37</v>
       </c>
       <c r="G12">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="9"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="5"/>
       <c r="F13" t="s">
         <v>39</v>
       </c>
       <c r="G13">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="9"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="5"/>
       <c r="F14" t="s">
         <v>40</v>
       </c>
@@ -1091,57 +1091,57 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="35" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="38" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="13"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B19">
@@ -1151,113 +1151,121 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f>-2250-800-60</f>
-        <v>-3110</v>
-      </c>
-      <c r="H19" s="15">
-        <v>0</v>
-      </c>
-      <c r="I19" s="15">
-        <v>0</v>
-      </c>
-      <c r="J19" s="15">
+        <f>G12*10+G13*10+G14</f>
+        <v>3210</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0</v>
+      </c>
+      <c r="J19" s="8">
         <v>-4063</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B20">
         <f>-D20*1.9</f>
-        <v>5795</v>
+        <v>-5985</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <f>-2250-800</f>
-        <v>-3050</v>
-      </c>
-      <c r="H20" s="15">
+        <f>G12*10+G13*10</f>
+        <v>3150</v>
+      </c>
+      <c r="H20" s="8">
         <v>5400</v>
       </c>
-      <c r="I20" s="15">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15">
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
         <v>-2845</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B21">
         <f>D21*1.5</f>
-        <v>-4575</v>
+        <v>4725</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <f>-2250-800</f>
-        <v>-3050</v>
-      </c>
-      <c r="H21" s="15">
+        <f>G12*10+G13*10</f>
+        <v>3150</v>
+      </c>
+      <c r="H21" s="8">
         <v>-4265</v>
       </c>
-      <c r="I21" s="15">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15">
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
         <v>-2845</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <f>-3050*2.2</f>
-        <v>-6710.0000000000009</v>
-      </c>
-      <c r="H22" s="15">
-        <v>0</v>
-      </c>
-      <c r="I22" s="15">
+        <f>-D22*2.2</f>
+        <v>-6930.0000000000009</v>
+      </c>
+      <c r="D22">
+        <f>G12*10+G13*10</f>
+        <v>3150</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
         <v>-6250</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="8">
         <v>-4240</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <f>3050*2.2</f>
-        <v>6710.0000000000009</v>
-      </c>
-      <c r="H23" s="15">
-        <v>0</v>
-      </c>
-      <c r="I23" s="15">
+        <f>D23*2.2</f>
+        <v>6930.0000000000009</v>
+      </c>
+      <c r="D23">
+        <f>G12*10+G13*10</f>
+        <v>3150</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0</v>
+      </c>
+      <c r="I23" s="8">
         <v>6250</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="8">
         <v>-4240</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B24">
@@ -1267,50 +1275,50 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f>-4*(2250+800)</f>
-        <v>-12200</v>
-      </c>
-      <c r="H24" s="15">
-        <v>0</v>
-      </c>
-      <c r="I24" s="15">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15">
+        <f>-4*D23</f>
+        <v>-12600</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8">
         <v>-11380</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
     </row>
     <row r="27" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E28" t="s">
@@ -1318,16 +1326,16 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E29" t="s">
@@ -1335,16 +1343,16 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="22" t="s">
         <v>33</v>
       </c>
       <c r="E30" t="s">

</xml_diff>

<commit_message>
SU/ST Cas de charges MECAmaster
Ya plus qu'à mettre dans l'excel
</commit_message>
<xml_diff>
--- a/SU_Suspension/05_Cas de charges/Cas de charges Valkyriz.xlsx
+++ b/SU_Suspension/05_Cas de charges/Cas de charges Valkyriz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\05_Cas de charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0102EA-54A5-4ABB-B3DD-A8F05C298C71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746775B3-8A72-4BE8-96FB-291D726D1A94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E17D21D-D292-4944-904A-D92C97BB235F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>CAS DE CHARGES VALKYRIZ ELIZ-2021</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Normal Force on RL Wheel =Normal force on FL Wheel</t>
   </si>
   <si>
-    <t>Y force on each exterior wheel = 2130</t>
-  </si>
-  <si>
-    <t>Y force on each interior wheel = 920</t>
-  </si>
-  <si>
     <t>RIGHT TURN 2,2G</t>
   </si>
   <si>
@@ -166,13 +160,91 @@
   </si>
   <si>
     <t>70/30</t>
+  </si>
+  <si>
+    <t>LEFT TURN 0,5 G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 0,5 G</t>
+  </si>
+  <si>
+    <t>LEFT TURN 1 G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 1 G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coeff de Frottement </t>
+  </si>
+  <si>
+    <t>BREAKING 1,9G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 1 G + BREAKING 1G</t>
+  </si>
+  <si>
+    <t>LEFT TURN 1,5 G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 1,5 G</t>
+  </si>
+  <si>
+    <t>LEFT  TURN 1 G + BREAKING 1G</t>
+  </si>
+  <si>
+    <t>LEFT TURN 1G + BUMP 1,5 G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 1 G + BUMP 1,5 G</t>
+  </si>
+  <si>
+    <t>Hypothèse</t>
+  </si>
+  <si>
+    <t>Normal Force on RR Wheel = Normal Force on RL Wheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Répartition de masse </t>
+  </si>
+  <si>
+    <t>Normal Force in R Inner Wheel = 0</t>
+  </si>
+  <si>
+    <t>LEFT TURN 1,8 G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 1,8 G</t>
+  </si>
+  <si>
+    <t>Suppose un coeff de frottement de  1,5</t>
+  </si>
+  <si>
+    <t>LEFT TURN 1,4 G</t>
+  </si>
+  <si>
+    <t>RIGHT TURN 1,4 G</t>
+  </si>
+  <si>
+    <t>Limite du modèle avec coeff à 1,4</t>
+  </si>
+  <si>
+    <t>La roue arrière intérieure ne touche plus le sol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cas limite </t>
+  </si>
+  <si>
+    <t>Normal Force F Inner Wheel = Normal Force on R Inner Wheel (Peut être condanable car on n'a pas une répartition 50/50 pour la masse)</t>
+  </si>
+  <si>
+    <t>Coeff de frottement sur la roue arrière extérieure = 1 selon x et y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -532,6 +604,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="20"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,8 +728,8 @@
       <xdr:rowOff>19275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1206484</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3514256</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>89761</xdr:rowOff>
     </xdr:to>
@@ -996,374 +1070,667 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D297AD9F-EA5F-4675-8006-39DF41B7B54A}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="3" width="31.109375" customWidth="1"/>
-    <col min="4" max="5" width="33.6640625" customWidth="1"/>
-    <col min="6" max="7" width="31.109375" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="67.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="B1" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:8" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
+    <row r="5" spans="1:8" ht="15" thickBot="1"/>
+    <row r="6" spans="1:8" ht="26.4" thickBot="1">
+      <c r="B6" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="16.8" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="16.8" customHeight="1">
+      <c r="F10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.8" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>230</v>
+      </c>
+      <c r="H11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="16.8" customHeight="1" thickBot="1">
       <c r="A12" s="3"/>
       <c r="F12" t="s">
         <v>37</v>
       </c>
       <c r="G12">
-        <v>230</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.8" customHeight="1" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="5"/>
       <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
         <v>39</v>
       </c>
-      <c r="G13">
-        <v>85</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:8" ht="16.8" customHeight="1" thickBot="1">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="5"/>
       <c r="F14" t="s">
         <v>40</v>
       </c>
-      <c r="G14">
-        <v>60</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="G14" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="16.8" customHeight="1" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="40"/>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.8" customHeight="1" thickBot="1">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="B16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="39"/>
-    </row>
-    <row r="17" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="37"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="41"/>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16.8" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="16.8" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="E18" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <f>G12*10+G13*10+G14</f>
+      <c r="B19" s="26">
+        <v>0</v>
+      </c>
+      <c r="C19" s="26">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26">
+        <f>G11*10+G12*10+G13</f>
         <v>3210</v>
       </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="8">
-        <v>0</v>
-      </c>
-      <c r="J19" s="8">
-        <v>-4063</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A20" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="26">
         <f>-D20*1.9</f>
         <v>-5985</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f>G12*10+G13*10</f>
-        <v>3150</v>
-      </c>
-      <c r="H20" s="8">
-        <v>5400</v>
-      </c>
-      <c r="I20" s="8">
-        <v>0</v>
-      </c>
-      <c r="J20" s="8">
-        <v>-2845</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
+      <c r="C20" s="26">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A21" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="26">
         <f>D21*1.5</f>
         <v>4725</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <f>G12*10+G13*10</f>
-        <v>3150</v>
-      </c>
-      <c r="H21" s="8">
-        <v>-4265</v>
-      </c>
-      <c r="I21" s="8">
-        <v>0</v>
-      </c>
-      <c r="J21" s="8">
-        <v>-2845</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="C21" s="26">
+        <v>0</v>
+      </c>
+      <c r="D21" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f>-D22*2.2</f>
+      <c r="B22" s="26">
+        <v>0</v>
+      </c>
+      <c r="C22" s="26">
+        <v>0</v>
+      </c>
+      <c r="D22" s="26">
+        <f>-4*D34</f>
+        <v>-12600</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A23" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="26">
+        <v>0</v>
+      </c>
+      <c r="C23" s="26">
+        <f>-D23*0.5</f>
+        <v>-1575</v>
+      </c>
+      <c r="D23" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="26">
+        <v>0</v>
+      </c>
+      <c r="C24" s="26">
+        <f>D24*0.5</f>
+        <v>1575</v>
+      </c>
+      <c r="D24" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A25" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="26">
+        <v>0</v>
+      </c>
+      <c r="C25" s="26">
+        <f>-D25*1</f>
+        <v>-3150</v>
+      </c>
+      <c r="D25" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A26" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="26">
+        <v>0</v>
+      </c>
+      <c r="C26" s="26">
+        <f>D26*1</f>
+        <v>3150</v>
+      </c>
+      <c r="D26" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A27" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="26">
+        <v>0</v>
+      </c>
+      <c r="C27" s="26">
+        <f>-D27*1.4</f>
+        <v>-4410</v>
+      </c>
+      <c r="D27" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A28" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="26">
+        <v>0</v>
+      </c>
+      <c r="C28" s="26">
+        <f>D28*1.4</f>
+        <v>4410</v>
+      </c>
+      <c r="D28" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A29" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="26">
+        <v>0</v>
+      </c>
+      <c r="C29" s="26">
+        <f>-D29*1.5</f>
+        <v>-4725</v>
+      </c>
+      <c r="D29" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A30" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="26">
+        <v>0</v>
+      </c>
+      <c r="C30" s="26">
+        <f>D30*1.5</f>
+        <v>4725</v>
+      </c>
+      <c r="D30" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="26">
+        <v>0</v>
+      </c>
+      <c r="C31" s="26">
+        <f>-D31*1.8</f>
+        <v>-5670</v>
+      </c>
+      <c r="D31" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="16.8" customHeight="1">
+      <c r="A32" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="26">
+        <v>0</v>
+      </c>
+      <c r="C32" s="26">
+        <f>D32*1.8</f>
+        <v>5670</v>
+      </c>
+      <c r="D32" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16.8" customHeight="1">
+      <c r="A33" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="26">
+        <v>0</v>
+      </c>
+      <c r="C33" s="26">
+        <f>-D33*2.2</f>
         <v>-6930.0000000000009</v>
       </c>
-      <c r="D22">
-        <f>G12*10+G13*10</f>
-        <v>3150</v>
-      </c>
-      <c r="H22" s="8">
-        <v>0</v>
-      </c>
-      <c r="I22" s="8">
-        <v>-6250</v>
-      </c>
-      <c r="J22" s="8">
-        <v>-4240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="D33" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="26">
+        <v>0</v>
+      </c>
+      <c r="C34" s="26">
+        <f>D34*2.2</f>
+        <v>6930.0000000000009</v>
+      </c>
+      <c r="D34" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="26">
+        <f>-D35</f>
+        <v>-3150</v>
+      </c>
+      <c r="C35" s="26">
+        <f>-D35*1</f>
+        <v>-3150</v>
+      </c>
+      <c r="D35" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="26">
+        <f>-D36</f>
+        <v>-3150</v>
+      </c>
+      <c r="C36" s="26">
+        <f>D36*1</f>
+        <v>3150</v>
+      </c>
+      <c r="D36" s="26">
+        <f>G11*10+G12*10</f>
+        <v>3150</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="26">
+        <v>0</v>
+      </c>
+      <c r="C37" s="26">
+        <f>-D36*1</f>
+        <v>-3150</v>
+      </c>
+      <c r="D37" s="26">
+        <f>(G11*10+G12*10)*2.5</f>
+        <v>7875</v>
+      </c>
+      <c r="E37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="26">
+        <v>0</v>
+      </c>
+      <c r="C38" s="26">
+        <f>D36*1</f>
+        <v>3150</v>
+      </c>
+      <c r="D38" s="26">
+        <f>(G11*10+G12*10)*2.5</f>
+        <v>7875</v>
+      </c>
+      <c r="E38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" thickBot="1">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" thickBot="1">
+      <c r="A48" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f>D23*2.2</f>
-        <v>6930.0000000000009</v>
-      </c>
-      <c r="D23">
-        <f>G12*10+G13*10</f>
-        <v>3150</v>
-      </c>
-      <c r="H23" s="8">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8">
-        <v>6250</v>
-      </c>
-      <c r="J23" s="8">
-        <v>-4240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="B48" s="28"/>
+      <c r="C48" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <f>-4*D23</f>
-        <v>-12600</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0</v>
-      </c>
-      <c r="I24" s="8">
-        <v>0</v>
-      </c>
-      <c r="J24" s="8">
-        <v>-11380</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="25" t="s">
+      <c r="D48" s="30"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27" t="s">
+      <c r="B49" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="28"/>
-    </row>
-    <row r="28" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="C49" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="D49" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="E49" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="14" t="s">
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E28" t="s">
+      <c r="B50" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
+      <c r="C50" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="E50" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="18" t="s">
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1">
+      <c r="A51" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E29" t="s">
+      <c r="B51" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="C51" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="D51" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="E51" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>

</xml_diff>